<commit_message>
Take average with 2 scores and redo the json
</commit_message>
<xml_diff>
--- a/data/Training.xlsx
+++ b/data/Training.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\gender-guesser\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72BC5FBE-86B5-4AE2-BCC7-EAAE8CD61664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D0750CD-6413-4D64-B9D8-3EDBECEF2277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="182">
   <si>
     <t>#</t>
   </si>
@@ -3295,687 +3295,11 @@
 by Joe Clark, the Bloc Quebecois led by Gilles Duceppe?"</t>
   </si>
   <si>
-    <t>Sabbath surfaces in Canadian election campaign.</t>
-  </si>
-  <si>
-    <t>OTTAWA, Nov 9 (Reuters) - The idea of a politician insisting on taking the Sabbath off, which arose with U.S. vice
-presidential nominee Joe Lieberman this summer, became a minor issue in the Canadian election campaign on
-Thursday.
-Liberal Prime Minister Jean Chretien took a poke, in remarks to reporters, at opposition leader Stockwell Day's
-habit of taking Sundays off during the five-week campaign.
-"Being prime minister is more than photo ops. It's a full-time job, even on Sunday," Chretien told reporters in
-reference to Day.
-That prompted a swift demand from Day's chief strategist, Rod Love, for an apology. "That was a disgraceful
-comment and the prime minister owes Stockwell Day an apology," Love told CTV television.
-Chretien spokeswoman Francoise Ducros declined to respond to Love's call.
-Day is an evangelical Christian and sat out the first day of the federal campaign, Oct. 22, because it was a
-Sunday. Lieberman, who is Jewish, follows a policy of taking Saturdays off, and maintained this as the
-Democratic candidate for vice president.</t>
-  </si>
-  <si>
-    <t>UPDATE 3-Canada's Chretien under fire in election debate.</t>
-  </si>
-  <si>
-    <t>OTTAWA, Nov 9 (Reuters) - Prime Minister Jean Chretien came under persistent heavy fire on Thursday night in
-the second and final televised debate of Canada's five-week campaign for the Nov. 27 federal election.
-Chretien, 66, who called the election early to try to gain a third successive parliamentary majority, faced withering
-attacks on everything from patronage and arrogance to health care cuts, but dished out his own retorts as well.
-The veteran Liberal leader looked uncomfortable as his opponents attacked him in the English debate. The night
-before, all four opposition party leaders ganged up on him in a French debate.
-"It's difficult, there's no doubt. When you're prime minister, there are four people who are attacking you," Chretien
-told reporters after the two-hour fracas.
-"If you can't handle big government, Mr. Chretien, perhaps you should stand aside," Canadian Alliance leader
-Stockwell Day, Chretien's biggest threat, had told him, referring to the alleged mismanagement of billions of
-dollars of job grants.
-"There's a great reluctance on the part of Mr. Chretien to go after the criminals," declared Day, who was able to
-land far more telling blows than he had been able to do in French, a language in which he is less comfortable.
-Joe Clark of the Conservative Party said Chretien had clearly been in office too long and abused his power by
-bringing questionable grants to his home district: "He thinks he made Canada the best country in the world all by
-himself.
-"Remember - he slashed health care and then built fountains in his riding (district) with your money because he
-thinks he can get away with anything," Clark said.
-But Chretien pushed the hot button of abortion in accusing Day of wanting to reopen a debate through a national
-referendum, noting referendums on Quebec separation had been divisive.
-"We have had two referendums. It is very, very divisive in a society, it breaks families and villages and
-communities. And you want in your programs to have referendums on everything that is controversial in the land,"
-Chretien said.
-"We have had peace on the abortion issue since the decision of the Supreme Court in 1988."
-Day, a conservative who wants to allow citizen-originated referendums as in California or Switzerland, said he
-opposes abortion but declared that was not Alliance policy.
-"The Canadian Alliance doesn't have a position on this particular topic, but we do have a position saying that if
-citizens want to discuss issues... they can be free to do it," he said.
-And Day attacked Chretien for having dared the separatists, during this campaign, to call a third referendum.
-Health care, provided by the government in Canada, is another hot issue given the deterioration of the system
-under spending cuts Chretien ordered to conquer fiscal deficits.
-Clark said the prime minister could not forever use the crutch of inherited deficits as an excuse for the cuts:
-"You're the guy who gutted the Canadian health system."
-Page 64 of 163 © 2021 Factiva, Inc. All rights reserved.
-Day, who has been accused of wanting to set up a two-tier health care system, held up a sign: "No two-tier health
-care."
-He then challenged Chretien to yank Liberal ads accusing him of favoring such a system, where the rich get
-quicker service. "Call me a liar or pull those negative U.S.-style ads," Day said.
-Chretien retorted: "Come clean with the Canadian people."
-Organizers of the debate criticized Day afterwards for having broken the rules by using a prop during the debate,
-but Day told reporters he had to get out the truth.
-The prime minister called the election on Oct. 22, only 3-1/2 years into his five-year mandate to counter the rise of
-the Alliance and capitalize on his standing in the polls.
-Before last month, Chretien had a 20-30 point lead in the polls. That shrank to 13-16 points by the end of
-October, but the most recent poll, released on Wednesday, gave Chretien a 22 percent lead over the Alliance.
-Part of Day's pitch has been that he is a fresh face with new ideas - a time for change - and he points to the fact
-that Chretien has been in federal politics for 37 years. "Where there is no vision, the people perish," he said.
-Chretien defended himself afterwards: "I have a lot of experience, that's true. (But) I'm still in very good shape."</t>
-  </si>
-  <si>
-    <t>Tempers set to flare in second Canada election debate.</t>
-  </si>
-  <si>
-    <t>OTTAWA, Nov 9 (Reuters) - Canada's prime minister and its main opposition leader were set for a ferocious
-sparring match in a televised debate on Thursday night that could go long way to deciding who will win the Nov.
-27 general election.
-Prime Minister Jean Chretien will try to use the English-language debate to portray Stockwell Day, leader of
-right-wing Canadian Alliance party, as an extremist who wants to destroy what Canadians hold dear.
-Day, whose low-tax, tough-on-crime party wants to transfer some of Ottawa's powers to Canada's 10 provinces,
-will accuse Chretien of presiding over a wasteful government that has consistently broken its promises.
-Chretien's Liberal party enjoys a healthy lead over the second-place Alliance in the polls.
-Canada's five party leaders battled to a draw on Wednesday night in a raucous yet inconclusive debate in French
-- Canada's other official language. The debate was not helped by the fact that only two participants were native
-francophones.
-The veteran 66-year-old Chretien said he was likely to use the second debate to press Day over whether the
-Alliance would allow binding referendums on such divisive issues as limiting abortion and restoring the death
-penalty.
-Senior Alliance member Diane Ablonczy, dismissing the French-language debate as "very boring", said on
-Thursday the real excitement would come in the second debate.
-"Tonight I think all the leaders will be on an equal footing and you'll see a lot more energy and a lot more
-controversy in this particular debate. I think a lot of people are looking forward to that," she said.
-Viewers will undoubtedly be expecting a better spectacle than the first debate where Day - whose grasp of the
-French language is shaky - chose to remain largely quiet and let the others savage Chretien over his
-government's record.
-"When you look at what happened tonight, with the sparks flying and some of the wrangling that was going on, I
-made a clear decision to stand back and let that happen," Day told reporters after the debate.
-The concerted attacks on Chretien overshadowed an almost ritual exchange between the prime minister and
-Gilles Duceppe, whose Bloc Quebecois party wants the French-speaking province of Quebec to break with
-Canada.
-The debates, which come halfway through the five-week campaign, can play a crucial role in influencing voters.
-The other parties taking part are the left-leaning New Democrats and the minority Conservatives, both fighting for
-survival.
-An Environics poll released on Wednesday showed the Liberals were now ahead of the Alliance by 48 percent to
-26 percent, up from the 45-29 spread registered by the same pollster last week.
-Day and Chretien will also attack each other over the sickly state of the country's state-funded healthcare system,
-still suffering from deep spending cuts the Liberals imposed in the mid-1990s to eliminate a huge budget deficit.
-Page 66 of 163 © 2021 Factiva, Inc. All rights reserved.
-Chretien says the Alliance is trying to set up a formal parallel private healthcare system, which is illegal under
-Canadian law. Day denies the charge and says the Alliance wants to put more money into medicare.
-Officials from his party last week suggested private-sector companies could help ease the burden by offering
-some services to patients, prompting Chretien to accuse Day of favoring one healthcare system for the rich and
-another for the poor.</t>
-  </si>
-  <si>
-    <t>UPDATE 3-Canadian PM savaged over health care cuts.</t>
-  </si>
-  <si>
-    <t>himself under heavy fire at the start of a leadership debate on Wednesday because of his Liberal government's
-cuts to the health care system.
-Chretien, who has been in power for seven years, said he had been forced to slash spending on Canada's
-state-funded "medicare" system in 1995 to cut a $27.3 billion ($42 billion Canadian) budget deficit left to him by
-the outgoing Conservatives.
-Canada's medicare system is the only health care provider in the country. It is much-loved here, but critics say it
-is underfunded.
-But four opposition leaders lined up to accuse Chretien of cynicism, noting that Chretien had signed a September
-deal with the country's 10 provinces to restore $14.3 billion ($22 billion Canadian) in health spending and then
-called the election almost immediately.
-"In reality it is you who have betrayed the legacy of Lester Pearson (the Liberal prime minister who introduced
-medicare in the mid-1960s) and the Liberals," thundered Joe Clark, leader of the minority Conservatives.
-"You are responsible for the problems in health care," he said during the opening half-hour of a noisy and testy
-French-language debate.
-This cut little ice with the 66-year-old Chretien, who is trying to win a third consecutive mandate and whose party
-is well ahead in the polls.
-"You left the country bankrupt and everyone in Canada had to tighten their belts," he replied, saying he had
-begun pumping money into the system as soon as he could. Opinion polls regularly show voters are most
-concerned about health care.
-Gilles Duceppe, leader of the separatist Bloc Quebecois party from French-speaking Quebec, also savaged
-Chretien over the medicare cuts and denounced the timing of the health care deal as as "cynical electoral ploy."
-Chretien tried to turn the tables on his opponents, accusing Canadian Alliance leader Stockwell Day of secretly
-seeking to set up a parallel private health care system alongside medicare, an idea many Canadians oppose.
-Day flatly denied the charges, saying the right-wing Alliance wanted to put more money into medicare. But the
-Alliance is also open to letting the government pay for medical procedures at private clinics.
-VOTERS AWAITED DEBATES
-The debates, which come half way through the five-week campaign, often play an important role in influencing
-voters. Only seven million of Canada's 30 million population speak French and the more important debate in
-English - Canada's other official language - takes place on Thursday.
-Chretien's hopes of victory were buoyed by an Environics poll released on Wednesday which showed the Liberals
-had widened their national lead over the Alliance, which is on the defensive over whether it would allow binding
-referendums on limiting abortion and restoring the death penalty.
-Page 68 of 163 © 2021 Factiva, Inc. All rights reserved.
-The Environics poll showed the Liberals were now ahead by 48 to 26 percent, up from the 45-29 spread
-registered by the same pollster last week.
-"It's one of the reasons we're looking forward to the debates today and tomorrow, so that Canadians can see and
-hear unfiltered from the leaders," Alliance strategist Rod Love told CBC television.
-The Conservatives and the minority left-leaning New Democrats are battling for survival in the election and are
-unlikely to feature highly in the debates.
-Day earlier tried to blast the Liberals on their financial accountability, but had to address apparent discrepancies
-between his party's official platform on referendums and policies set out in a party manual for candidates.
-The manual suggests a petition signed by 3 percent of voters - fewer than 400,000 people - would be enough to
-force a binding referendum on any issue. That would include such potentially divisive issues as abortion and
-capital punishment.
-The Alliance's official policy platform, on the other hand, does not specify how many signatures would be needed
-to trigger a referendum. Day suggested on Wednesday that a 3 percent threshold may be too low. (Additional
-reporting by Robert Melnbardis in Montreal).</t>
-  </si>
-  <si>
-    <t>UPDATE 1-Canadian PM savages opposition over gun control.</t>
-  </si>
-  <si>
-    <t>OTTAWA, Nov 6 (Reuters) - Canada's low-key election race roared into life on Monday when Prime Minister Jean
-Chretien claimed that a vote for the main opposition party on Nov. 27 could leave the low-crime country awash
-with firearms.
-Chretien, denying that he was launching a personal attack on Canadian Alliance leader Stockwell Day,
-nevertheless attacked his right-wing opponent over a vow to scrap the government's tough 1995 gun control
-legislation.
-"This law is very, very important for Canadians and I want them to know that if they vote for Stockwell Day there is
-a chance that people will be able to buy firearms at will as they can in certain U.S. states," Chretien told reporters
-after a speech to members of his ruling Liberal Party in Ottawa.
-Day says that if he wins the election he will scrap the gun control law, which was enacted after a lone gunman
-killed 14 young women in a Montreal school in 1989.
-Chretien, reminding his audience that firearm homicide rates in the United States are more than eight times
-higher than those in Canada, said the legislation was one of his government's great achievements.
-Canada prides itself in having far fewer violent crimes than its southern neighbour and the gun control debate
-goes to the heart of the country's national identity. There are 250 million firearms in the United States, almost one
-for each person, compared to 7 million for 30 million Canadians.
-One main plank of the 1995 law is a costly gun registration scheme which requires the listing of all firearms.
-Previously only handguns had to be registered.
-The scheme is very unpopular in western provinces such as Alberta - Day's main power base - where people see
-it as an infringement of their human rights.
-OPPOSITION SAYS GUN CONTROL LAW IS "A DISASTER"
-"(The gun control law) is a disaster. It will not reduce crime," Day said in an interview broadcast over the Internet
-on Monday. The Alliance says given that criminals are unlikely to register their guns, the only way to clamp down
-on crime is to hire more police to enforce existing laws.
-Day and Chretien are likely to resume their attacks in two televised leadership debates this Wednesday and
-Thursday.
-Chretien - seeking to paint Day as an extremist who will destroy Canada's generous social programmes and the
-country's communitarian spirit - also repeated his assertion that an Alliance win would mean the right of Canadian
-women to have abortions could be strictly curtailed.
-Canada's right-wing parties - the Alliance and the minority Conservatives - have sharpened their electoral
-offensive after opinion polls showed the Liberals 13-16 points ahead after the first two weeks of the five-week
-campaign.
-Day - under pressure from his advisors to drop his so-called "agenda of respect" and attack Chretien - on
-Saturday said the prime minister had been corrupted by the amount of power he had amassed since taking power
-in 1993.
-Page 70 of 163 © 2021 Factiva, Inc. All rights reserved.
-Earlier on Monday, Day highlighted what he said were Chretien's many broken promises.
-"These are things which stand as an indictment of this government," he told a news conference.
-The Conservatives also stepped up a gear on Monday, releasing anti-Chretien television adverts which took the
-form of a spoof on commercials for CDs.
-"Here it is Canada! Jean Chretien's Greatest Lies. All 101 over the last seven years on one disc," said one advert,
-referring to Chretien's reversals on issues such as free trade and eliminating a national sales tax.
-Chretien - who called the election less than 3-1/2 years into his second five-year mandate to capitalise on his
-opinion poll lead - declined to comment when asked about the adverts.
-(With additional reporting by Randall Palmer in Ottawa).</t>
-  </si>
-  <si>
-    <t>Attacks fly in Canadian election campaign.</t>
-  </si>
-  <si>
-    <t>OTTAWA, Nov. 7 (Reuters) - The leader of the Canadian Alliance, seeking to oust the Liberals in a Nov. 27
-election, charged Prime Minister Jean Chretien on Tuesday with running a campaign of fear and smear.
-In a campaign where each side increasingly accuses the other of going negative or getting personal, Alliance
-leader Stockwell Day said Chretien had consistently misrepresented the Alliance's campaign to make government
-accountable.
-"He has been wrong on areas of Alliance policy time after time. He throws out the fear and smear to the Canadian
-public - (and is) absolutely wrong on Canadian Alliance policy - because he doesn't want to talk about his policy,"
-Day told a news conference.
-Day has cut Chretien's lead in the polls to 13-16 percentage points from the 19-32 points it stood at before
-Chretien called the election on Oct. 22, although polls still indicate that Chretien should win an overall majority.
-Chretien, also wounded by Progressive Conservative ads that call him a liar, says his rivals' shift to attack mode
-reflects the fact that their poll ratings are not improving.
-"They don't talk about their platform any more. They have moved to name-calling, to character assassination. It is
-not my style of politics but I predict it might get a bit worse," he told a Liberal rally on Monday night.
-"I was in politics with (former prime minister) Mike (Lester) Pearson, who was a great gentleman and was subject
-to that kind of politics once in a while. I remember the words he used. He used to say that those who threw mud
-lost ground.
-"We won't attack them personally. We'll attack the kind of society they want to build in Canada."
-But at the same time Chretien lashed out at Day for his pledge to scrap a 1995 law that requires all guns to be
-registered. Day says it will not reduce crime and only draws police off the streets.
-Chretien accused Day of having bought a gun on the day the bill was passed. In fact, Day bought it a year earlier,
-on the day the gun legislation was introduced in Parliament.
-FIRST REAL THREAT TO LIBERALS
-Day is providing the first real threat to Chretien's grip on power from outside his own Liberal party since the
-Liberals came to power in 1993. His party, a grass-roots organisation originating in western Canada, is dedicated
-to tax cuts and reducing the size of government.
-The Alliance has also pledged to allow citizen's initiatives on social issues similar to those in California or
-Switzerland, and says it will consult on the number of signatures needed to launch one.
-A manual for Alliance candidates, which came to light on Tuesday, says the party proposes a threshold of 3
-percent of those who voted in the last election - which would mean around 400,000 of Canada's 30 million people.
-Day, stressing his personal belief that that life begins at conception, said he felt 3 percent was too low a
-threshold.
-Page 72 of 163 © 2021 Factiva, Inc. All rights reserved.
-Abortion has been legal since the Supreme Court struck down federal legislation in 1988, and the Liberal Party
-charged on Tuesday that Day was trying "to cover up his own willingness to trigger divisive referenda on issues
-like abortion."
-On a separate tack, Chretien sent regrets late on Monday night to Canada's Jewish community, which has often
-voted Liberal but which has looked askance at a Canadian vote at the United Nations on the Israeli-Palestinian
-violence and has also looked favourably at Day's support for religious schools.
-Speaking of frustration that the Israeli government's "courageous compromises" have not been reciprocated,
-Chretien wrote: "We regret that Canada's vote on U.N. Security Council Resolution 1322 has added to this
-distress and frustration."</t>
-  </si>
-  <si>
-    <t>Canadian leaders gear up for tough election debates.</t>
-  </si>
-  <si>
-    <t>OTTAWA, Nov 7 (Reuters) - All five leaders vying for the top crown in Canada's election will crowd the stage in
-two leadership debates this week, a process that will sorely test the stamina of the 66-year-old prime minister,
-Jean Chretien.
-The veteran Liberal Party leader, trying to win a third consecutive majority mandate on Nov. 27, could be in for a
-pummeling in both the French-language debate on Wednesday and the crucial English-language debate on
-Thursday.
-"It is going to be tougher for the prime minister than the others since everyone will be gunning for him on both
-nights," said one Chretien aide.
-The somewhat unwieldy debates - which feature all five leaders on the same stage - come halfway through the
-five-week run-up to the election and traditionally mark the point where voters start paying serious attention to the
-campaign.
-By far the most important debate comes on Thursday, which is likely to be dominated by Chretien's battle with
-Stockwell Day, the 50-year-old leader of the opposition right-wing Canadian Alliance.
-Day - who says Canada desperately needs a new face running the country - is promising to hammer away at
-Chretien over what he says is the prime minister's arrogance, excessive secrecy, his broken promises and
-Ottawa's wasteful spending.
-"These are things which stand as an indictment against this government, these are things he does not want to talk
-about but I will be talking about these things," said Day, who spent 14 years honing his debating skills in the
-Alberta government.
-Day, whose fledgling Alliance is trailing the Liberals nationally by around 15 points in the opinion polls, knows he
-has to sell himself to Canadians who have heard Chretien brand him as a right-wing extremist.
-The enormously experienced Chretien says if Day wins, the Alliance will partially privatise the state-funded health
-care system, scrap tough gun control laws and encourage a binding referendum on whether to clamp down on
-abortions.
-Chretien will also come under fire from the other two national parties - the minority Conservatives and the
-left-leaning New Democrats - which have been increasingly marginalized by the Liberal-Alliance fight for
-dominance.
-This might work to his advantage, since if the Alliance attacks him for not cutting taxes enough and the New
-Democrats accuse him of slashing them too far, it should be easier for Chretien to portray his approach as the
-most balanced.
-The Liberals are taking Day much more seriously than they ever did Preston Manning, the somewhat owlish
-leader of the Reform Party - the Alliance's predecessor.
-"The important thing is not to mess this up. We think we will be going into the English-language debate as slight
-underdogs," the Chretien aide said.
-Page 74 of 163 © 2021 Factiva, Inc. All rights reserved.
-"Day is much more telegenic than Manning ever was, he's a debater, he spent all those years in a legislature,
-which Manning never did. We hope he will be better than Manning."
-For Chretien, who visibly tired toward the end of his second week campaigning, it will be the second important
-face-to-face encounter in two nights.
-In the first televised clash he must try to persuade voters in French-speaking Quebec to back his ruling Liberals
-rather than the Bloc Quebecois of Gilles Duceppe, which advocates separation from Canada.
-The Conservatives and New Democrats - both bit players in Quebec - are unlikely to score many points in the
-debate.
-While the Alliance stands no chance of winning any seats in Quebec, Day will try to persuade French-speaking
-voters that he is much more friendly towards them than the vehemently anti-separatist Reform ever was.
-The debates are not always necessarily where a party can either win or lose an election. In the 1988 debate
-Liberal leader John Turner bettered Conservative leader Brian Mulroney but still lost the subsequent election.
-"Look at 1988. Who won the debate? We did. Who was ahead in the polls afterward? We were. We smoked
-them. And then they came back at us, attacked us mercilessly, regained their position in the polls and won," said
-the Chretien aide</t>
-  </si>
-  <si>
-    <t>Canadian PM's election campaign stuck in second gear.</t>
-  </si>
-  <si>
-    <t>OTTAWA, Nov 6 (Reuters) - Canadian Prime Minister Jean Chretien's campaign to win a Nov. 27 election seems
-stuck in low gear, with the veteran leader meandering through some of his speeches and showing signs of deep
-tiredness at the end of the second week.
-Despite travelling from east to west and back again, Chretien has had virtually no contact with ordinary voters,
-preferring instead to deliver much the same address two or three times a day, mainly to meetings of his Liberal
-Party.
-But even when faced with audiences guaranteed to be friendly the 66-year-old prime minister - with 37 years in
-federal politics - has looked distracted and unfocused.
-On Saturday he looked exhausted as he gave one of his least polished performances of the week before a crowd
-of party workers in Prince Edward Island.
-He stumbled through the speech, managing at one point to turn local literary heroine Anne of Green Gables into
-"Anne Gable", and had to ask someone to remind him of the name of a major local factory he had just visited.
-The main planks of a traditional campaign - addressing huge outdoor crowds, making speeches on the stump to
-win over undecided voters, chatting with reporters over a beer at the end of the day - have been notably absent.
-"This isn't a campaign, this is a business trip," sighed one veteran journalist who has covered Canadian elections
-for the last 25 years. But the prime minister still has a sizable lead in the polls which if translated into actual votes
-would give him a third successive majority government.
-His low-key approach is all the more surprising given that Liberal insiders had said Chretien was "really pumped
-up" by the prospect of taking on Stockwell Day, leader of the main opposition party, the right-wing Canadian
-Alliance.
-So far he has managed to avoid the mistakes of the 1997 election campaign when friend and foe alike
-acknowledge that his performance over the first 10 days - a time when aides say he was tired and ill - was a
-disaster which helped cut his majority in Parliament.
-CHRETIEN HAS LEGENDARY TENDENCY TO MAKE GAFFES
-And while Chretien is now keeping a tight grip on a legendary tendency to make gaffes, his renowned combative
-style is revealing itself only in short bursts. More noticeable is how tired the 66-year-old leader has often looked.
-"We made clear before the start of the campaign that he could not be allowed to do more than three events a day
-and we've stuck to that," said one Chretien aide.
-Yet despite this, another insider admitted: "It's the end of week two and we are all shattered."
-The dynamic 50-year-old Day - still looking fresh after making up to six campaign stops a day, sometimes
-sparring with vocal protesters - says Canada desperately needs a new face to replace what he says is a tired,
-uninspired prime minister.
-And although Chretien portrays himself as the only man experienced enough to lead Canada into the 21st
-century, his age is clearly a very sensitive topic.
-Page 76 of 163 © 2021 Factiva, Inc. All rights reserved.
-As he ran up the steps to his aircraft after a campaign stop on Saturday, the prime minister stumbled badly. A top
-aide told television crews that if they used the footage, their access to Chretien would be restricted.
-Other officials quickly intervened to apologise, but the results were predictable - the main television news
-programme that evening showed repeated shots of the Chretien slip. Other more metaphorical stumbles marked
-that Saturday.
-Chretien earlier addressed a party meeting in the high unemployment province of New Brunswick, where
-everyone was expecting him to mention the deep cuts in jobless benefits which cost the party dearly in the 1997
-election.
-But much to the surprise of the audience, Chretien did not address the topic at all and only realised his slip when
-prompted afterward by one of his candidates.
-"I wanted to talk about it, I forgot, I'm not perfect, I admit it," he said in French with a sheepish smile. Yet minutes
-later, speaking in English, he claimed he had deliberately skipped the subject.
-From now on, things are only going to get tougher.
-This week Chretien has two tough party leader debates and must then embark on what staffers say will be a
-frantic last fortnight, crisscrossing what is the world's second-largest country and working 18 hours a day.</t>
-  </si>
-  <si>
-    <t>Gloves come off in Canadian election campaign.</t>
-  </si>
-  <si>
-    <t>party aired attack ads slamming the "lies" of Prime Minister Jean Chretien and another lashed out at Chretien's
-arrogance and broken promises.
-Opposition leader Stockwell Day peeled the paper off the cover of an imitation of the Liberals' Red Book political
-platform to reveal what he said were broken promises from Chretien, who is seeking his third parliamentary
-majority in the Nov. 27 election.
-"These are things which stand as an indictment of this government," Day told a news conference. "There has
-probably been not a longer string of broken promises in Canadian history in government."
-Canada's right-wing parties - Day's Canadian Alliance and the Progressive Conservatives - have sharpened their
-electoral offensive after opinion polls showed the Liberals 13-16 points ahead after the first two weeks of the
-five-week campaign.
-Hardest-hitting are television ads from the once-ruling Conservatives, who are fighting for survival and for media
-play. The ads, a spoof on commercials for CDs, began airing on Monday.
-"Here it is Canada! Jean Chretien's Greatest Lies. All 101 over the last seven years on one disc," one ad says,
-referring to Chretien's reversals on issues such as free trade and eliminating a national sales tax. "It's the greatest
-pack of lies ever sold! And for the price of a $200 million election you get to listen to more lies!"
-Day at the weekend toughened his message to suggest Chretien had been tainted by his seven years in power.
-Chretien - who in the past has gone as far as to attack Day's evangelical Christianity - accused the Alliance leader
-on Sunday of abandoning what Day terms his agenda of respect.
-"We might have disagreements with people on policies, but so much for the agenda of respect. I have a record. I
-stand by it - public life has been my life and to have innuendoes of that nature is completely unacceptable," said
-Chretien, who had no day-time appearances on Monday.
-Day responded: "It is not disrespectful for the leader of the opposition to do as I have been doing and very
-aggressively pointing out the wrongdoings and how Canadians have been hurt by the federal Liberals."
-POWER ELITE
-Day denied a suggestion that he had attacked Chretien's family in referring to the "power elite" and the "power
-corporation" around Chretien.
-Chretien's daughter France, who is accompanying him on the campaign, is married to Andre Desmarais,
-chairman of the financial services conglomerate Power Corp. And a top Chretien strategist is Power Corp.
-executive vice president John Rae.
-"I've been saying for four months, I'm talking about a power elite in the prime minister's office, and I've compared
-him to a corporation. If he had been a CEO of any corporation, with his record of mismanagement, he would have
-been fired out the door," Day said.
-Page 78 of 163 © 2021 Factiva, Inc. All rights reserved.
-Chretien called the Nov. 27 election, less than 3-1/2 years into this five-year mandate, to capitalise on what had
-been a lead of 20 to 30 points in the polls.
-He has sought to paint Day as an extremist who will destroy Canada's generous social programmes, and on
-Sunday he reminded a crowd of women of Day's opposition to abortion. Canada has not had any restrictions on
-abortion since 1988.
-As provincial finance minister in Alberta, Day opposed government funding of abortions, but the Alliance has
-studiously avoided the divisive topic, while pledging to let citizens launch referendums on whatever topics they
-choose.
-"We have been very clear all along that abortion is not even on the platform of this party," said Day, who is more
-conservative than the Conservatives but who has sought to end the vote-splitting on the right in order to bring in
-smaller government and deeper tax and debt reductions.
-The area of the country where Day is weakest is in Quebec. A poll released on Monday put the Liberals dead
-even there at 43 percent with the Bloc Quebecois, which wants to take the mainly French-speaking province out
-of Canada.</t>
-  </si>
-  <si>
-    <t>UPDATE 2-Canadian Alliance cuts Liberal lead further.</t>
-  </si>
-  <si>
-    <t>OTTAWA, Nov 2 (Reuters) - The right-wing Canadian Alliance has further narrowed the gap with Prime Minister
-Jean Chretien's Liberal Party in the country's five-week federal election campaign, two new polls showed on
-Thursday.
-The Liberals probably still have enough support to win a third parliamentary majority on Nov. 27 if their power
-base does not continue to erode, but recent polls have shown growing momentum in favour of the the Alliance.
-An Ipsos-Reid poll released on Thursday night by CTV news showed that support for the Liberals had slipped
-slightly since the first week of the election campaign, while numbers for the Alliance had steadied.
-The poll, which was conducted Oct. 26 to Nov. 1 for CTV and the Globe and Mail, showed the Liberals at 42
-percent, down 3 percentage points from 45 percent in an Ipsos-Reid survey taken Oct. 19 to 25. The survey
-showed the Alliance at 29 percent, up 1 point.
-The Ipsos-Reid poll surveyed 2,500 voters and its national results are considered accurate to 2 percentage
-points. In an interview with CTV News, Ipsos-Reid pollster Darrell Bricker said the survey revealed continued
-erosion of support for the Liberals.
-"What we've seen is that they've lost a total of 10 points over the past three weeks," Bricker said.
-Earlier on Thursday, an Environics Research Group poll showed the Liberals ahead at 45 percent to the Alliance's
-29 percent in the period from Oct. 26 to 30. That compares with a 44 percent to 25 percent spread in Environics'
-previous poll, conducted Sept. 25 to Oct. 16.
-Environics said the other two national parties, the Conservatives and the leftist New Democrats, dropped to 7
-percent each from 9 percent and 10 percent respectively.
-"It's setting the stage for one of the most polarised campaigns we've seen in this country," Environics pollster
-Chris Baker told CBC television.
-Bricker said that like other polls, the Ipsos-Reid poll showed an east-west split in the country, with those provinces
-west of Ontario solidly behind the Alliance, and those east of Ontario backing the Liberals. The notable exception
-was French-speaking Quebec, where the polls showing the Liberals in a tight race with the separatist Bloc
-Quebecois.
-In the key battleground of Ontario, with more than one-third of the seats in the House of Commons, the gap has
-narrowed to 55 percent for the Liberals to 29 percent for the Alliance, from 56 percent and 22 percent, according
-to the Environics poll. The Ipsos-Reid survey had the Liberals up 2 points to 53 percent, and the Alliance down 4
-points to 24.
-Baker said Alliance support was not yet concentrated enough in Ontario to pick up more than a handful of seats.
-The Environics poll had the Alliance, with 14 percent, displacing the New Democrats in third place in the Atlantic
-region. But the Alliance still lagged the Liberals' 55 percent and the Conservatives' 22 percent. The New
-Democrats were at 9 percent.
-In Quebec, Environics had the Liberals tied at 45 percent with the Bloc Quebecois. But because Liberal support is
-concentrated in Montreal, the Bloc is expected to retain a majority of Quebec's seats.
-Page 80 of 163 © 2021 Factiva, Inc. All rights reserved.
-The Ipsos-Reid survey had the Bloc leading in Quebec, however, with a 43 percent share, up 6 points, and the
-Liberals at 38 percent, down 5 points
-The Environics poll surveyed 1,339 voters, a sample size that should give the same national result, plus or minus
-2.7 percentage points, 19 times out of 20.
-It was conducted over the end of the first week of the campaign but before Alliance campaign co-chairman Jason
-Kenney made headlines by talking about the possibility of a greater role for private health care in the country's
-public health system - a sensitive issue for most Canadians.</t>
-  </si>
-  <si>
-    <t>UPDATE 4-Canada's Liberals, opposition clash over healthcare.
-By David</t>
-  </si>
-  <si>
-    <t>OTTAWA, Nov 1 (Reuters) - Canadian Prime Minister Jean Chretien and opposition leader Stockwell Day on
-Wednesday exchanged bitter blows over the future of the state-funded healthcare system, which is rapidly
-becoming one of the key issues in the run-up to a Nov. 27 general election.
-Chretien promised his ruling Liberals would defend the country's cherished yet creaking medicare system against
-what he said were the efforts of Day's right-wing Canadian Alliance to introduced privatised health care.
-While the Alliance's official policy is to put more money into the system, key party officials have suggested this
-week that private-sector companies could help ease the burden by offering some services to patients.
-Chretien seized on what he said was the Alliance's hidden agenda and charged that Day wanted to introduce a
-private health care system for those who could afford it.
-"We will fight them. We don't want one healthcare system in Canada for the rich and one for the poor. It's not the
-Canadian way," he told a fundraising dinner in Ottawa.
-"The response of Canadians and Liberals to this hidden agenda is very clear - never, never, never, no way,"
-thundered the 66-year-old prime minister, who says an Alliance victory would produce a "winner-takes-all" society
-and cripple Canada's communitarian spirit.
-But Day, speaking at a dinner in Calgary, denied he wanted to hurt medicare and pointed out that the Liberals
-had only just agreed to restore the roughly C$20 billion in spending cuts they imposed in 1995 to eliminate a large
-budget deficit.
-"It is the Chretien government which has threatened medicare in this country. It is the Chretien government which
-has increased waiting lists," he said, denouncing what he said was the government's scare tactics.
-"So for them to come along after five years of cuts and start throwing accusations at those people who want to fix
-the system which they (the Liberals) broke is simply insulting to Canadians."
-Without giving details Day then went on to say the Alliance approach might mean "innovation, experimentation
-and flexibility in service delivery" but vowed patients would not pay extra for essential medical services.
-It remains to be seen whether the low-tax, tough-on-crime and anti-big government Alliance can get its message
-across to voters, who consistently say the future of medicare is their most pressing concern.
-The ballooning argument over healthcare overshadowed the Liberals' release on Wednesday of their election
-platform, in which they promised billions of dollars in extra spending.
-On top of tax cuts already pledged, the Liberals are promising C$6.6 billion ($4.3 billion) in new spending over the
-next four years on education, research and development, the environment, crime prevention and housing.
-The plan is long on rhetoric but short on details, at least in part because over the last two months the Liberals
-have announced the main planks of their platform.
-In September, Chretien hammered out a deal with Canada's 10 provinces to pump C$18.9 billion into the public
-health system over the next five years. And last month Ottawa announced C$100 billion worth of tax cuts over the
-same period and vowed to pay down the national debt at a faster rate.
-Page 82 of 163 © 2021 Factiva, Inc. All rights reserved.
-The Alliance also proposes massive tax cuts, as well as the transfer of some of Ottawa's powers to the 10
-provinces.
-Chretien, who has been in power for seven years, brushed off suggestions that he and his party were tired and
-running out of ideas.
-"We have plenty of ideas. Read this programme and compare it with anybody else's. There is more to life than
-taxes and taxpayers," he said forcefully.</t>
-  </si>
-  <si>
-    <t>UPDATE 1-Canadian Alliance cuts Liberal lead further.</t>
-  </si>
-  <si>
-    <t>Jean Chretien's Liberal Party in the country's five-week federal election campaign, a new poll showed on
-Thursday.
-The Liberals probably still have enough support to win a third parliamentary majority on Nov. 27 if their power
-base does not continue to erode, but recent polls have shown growing momentum in favour of the the Alliance.
-The Environics Research Group poll showed the Liberals ahead at 45 percent to the Alliance's 29 percent in the
-period from Oct. 26 to 30. That compares with a 44-25 percent spread in Environics' previous poll, conducted
-Sept. 25 to Oct. 16.
-And the other two national parties, the Conservatives and the leftist New Democrats, dropped to 7 percent each
-from 9 and 10 percent respectively.
-"It's setting the stage for one of the most polarised campaigns we've seen in this country," Environics pollster
-Chris Baker told CBC television.
-In the key battleground of Ontario, with more than one-third of the seats in the House of Commons, the gap has
-narrowed to 55 percent for the Liberals to 29 percent for the Alliance, from 56 and 22 percent.
-Baker said Alliance support was not yet concentrated enough in Ontario to pick up more than a handful of seats.
-In a surprise, the Alliance, with 14 percent, displaced the New Democrats in third place in the Atlantic region,
-though still lagged the Liberals' 55 percent and the Conservatives' 22 percent. The New Democrats were at 9
-percent.
-In Quebec, the Liberals were tied at 45 percent with the separatist Bloc Quebecois. But because Liberal support
-is concentrated in Montreal, the Bloc is expected to retain a majority of Quebec's seats.
-The poll surveyed 1,339 voters, a sample size that should give the same national result, plus or minus 2.7
-percentage points, 19 times out of 20.
-It was conducted over the end of the first week of the campaign but before Alliance campaign co-chairman Jason
-Kenney made headlines by talking about the possibility of a greater role for private health care in the country's
-public health system - a sensitive issue for most Canadians.
-Four other polls issued last Friday and Saturday had shown a Liberal lead of 17 to 20 points, but the survey
-periods ended either on Oct. 25 or 26. This was the first survey to cover a later time frame.
-The results also showed the number of undecided voters has nearly doubled to 19 percent from 10 percent in the
-earlier Environics survey.</t>
-  </si>
-  <si>
-    <t>Canadian Liberal platform attacked as costly sequel.</t>
-  </si>
-  <si>
-    <t>OTTAWA, Nov 2 (Reuters) - Why is Canadian Prime Minister Jean Chretien's reelection platform like a film
-sequel? Well, according to opposition leader Stockwell Day on Thursday, it's worse than the original and more
-expensive.
-Party strategists rushed out the platform, known as the Red Book for the colours of Chretien's governing Liberal
-party, after Chretien called the early Nov. 27 election to take advantage of a good standing in opinion polls.
-Released on Wednesday, it is the Liberals third Red Book, produced for elections in 1993 and 1997, which it won
-with majority governments. Some newspapers on Thursday nicknamed the new version "Red Book Lite."
-"Like the film versions, the sequels continue to disappoint. We had the Red Book, and then we had the sequel to
-that, and then just as we thought our wallets were safe, we now have Red Book III," Day, leader of the right-wing
-Canadian Alliance, said in a news conference televised from Calgary.
-"Some people have suggested a theme...for the Red Book III could be Jaws, because in fact this particular
-approach of the federal Liberals is going to take a huge bite out of our wallets and out of our purses."
-In unveiling the platform, Chretien pledged to maintain a 50-50 formula to roughly match new spending and and
-new debt and tax cuts.
-With C$100 billion ($65 billion) in tax cuts already pledged and about C$30 billion in new spending in the Red
-Book, Chretien said that would mean C$70 billion in spending still unaccounted for.
-BLANK CHECK
-"It appears as though the prime minister is asking for a blank check from Canadians as he goes into this next
-election," Day said.
-For Day, the focus on the Liberal platform was a welcome diversion from the latest attention on whether the
-Alliance would introduce two-tier health care - with private care supplementing the current policy of free public
-care.
-"I say to the prime minister: Go on the facts. Don't try scare tactics. Get away from that business of the two-tier
-smear and just go on the facts," he said.
-"We are committed to increase in health care (spending)," he said, adding that the Alliance wants to make it
-illegal for future governments to slash health spending as the Liberals did in the mid-1990s.
-Chretien did not mention health care during a tour of a carpentry training centre in Toronto on Thursday but
-defended his government against Alliance attacks on a "billion-dollar boondoggle" at the federal Human
-Resources Department over its alleged mismanagement of huge job creation grants.
-"We think the government can be a force for good in society and sometimes governments have to intervene to
-make the country move forwards," he said to cheers from unionized workers who have in the past traditionally
-voted for the left-wing New Democratic Party (NDP).
-But the NDP is being squeezed out by the Liberals and the Alliance, and Ucal Powell, secretary-treasurer for the
-Central Ontario Regional Council of Carpenters, made it quite clear Chretien had his vote.
-Page 85 of 163 © 2021 Factiva, Inc. All rights reserved.
-"Absolutely the (job creation) grants work. We have a shortage of skilled carpenters and the only way we are
-going to get them is to train apprentices and we need government support on that," he told reporters.
-"Anything that brings young Canadians to get meaningful jobs can never be a boondoggle. On this issue we feel
-very emotional."
-Chretien's Liberals maintain a lead of about 20 percentage points in the polls, enough to win a third straight
-majority in Parliament if translated into votes. But the last series of polls showed that the is gap narrowing.
-(Additional reporting by David Ljunggren in Toronto).</t>
-  </si>
-  <si>
-    <t>Canadian Alliance cuts Liberal lead further.</t>
-  </si>
-  <si>
-    <t>OTTAWA, Nov 2 (Reuters) - The right-wing Canadian Alliance has further narrowed the gap with Prime Minister
-Jean Chretien's Liberal Party in the country's five-week federal election campaign, a new poll showed on
-Thursday.
-The Liberals probably still have enough support to win a third parliamentary majority on Nov. 27 if their power
-base does not continue to erode, but recent polls have shown growing momentum in favour of the the Alliance.
-The Environics Research Group poll showed the Liberals ahead at 45 percent to the Alliance's 29 percent in the
-period from Oct. 26 to 30. That compares with a 44-25 percent spread in Environics' previous poll, conducted
-from Sept. 25 to Oct. 16.
-And the other two national parties, the Conservatives and the leftist New Democrats, dropped to 7 percent each
-from 9 and 10 percent respectively.
-"It's setting the stage for one of the most polarised campaigns we've seen in this country," Environics pollster
-Chris Baker told CBC television.
-In the key battleground of Ontario, with more than one-third of the seats in the House of Commons, the gap has
-narrowed to 55 percent for the Liberals to 29 percent for the Alliance, from 56 and 22 percent.
-Baker said Alliance support was not yet concentrated enough in Ontario to pick up more than a handful of seats,
-but Alliance strategist Line Maheux said the party could realistically win 12 to 20 of the province's 103 seats.
-And, in a surprise, the Alliance has now displaced the New Democrats in third place in the Atlantic region, with 14
-percent, though still behind the Liberals' 55 percent and the Conservatives' 22 percent. The New Democrats were
-at 9 percent.
-The poll surveyed 1,339 voters, a sample size that should give the same national result, plus or minus 2.7
-percentage points, 19 times out of 20.
-It was conducted over the end of the first week of the campaign but before Alliance campaign co-chairman Jason
-Kenney made headlines by talking about the possibility of a greater role for private health care in the country's
-public health system - a sensitive issue for most Canadians, who support the public system.</t>
-  </si>
-  <si>
-    <t>UPDATE 1-Health care now key Canada election issue.</t>
-  </si>
-  <si>
-    <t>OTTAWA, Nov 1 (Reuters) - After being a sleeper in the first week of the election campaign, the issue dear to
-most Canadian hearts - health care - surged to the fore this week.
-The governing Liberals' main challenger, the right-wing Canadian Alliance party, found itself on Wednesday
-having to defend against charges that it would allow a two-tier system, where those who can afford it can get
-speedier treatment.
-Pollsters and politicians alike know health is a hot button in any Canadian campaign, and Chretien with an eye to
-slippage in the polls was quick to cast himself as a saviour to the country's government-funded system.
-"It is one health care system for the rich and one for the rest of us," Prime Minister Jean Chretien said on
-Wednesday of the Alliance's plan. "Equal access to high-quality health care is a fundamental Canadian value."
-Most health care in Canada is free to everyone, unlike in the United States, where the government only funds
-care for the poor and for seniors.
-But the Canadian system is creaking under budget cuts and soaring costs. Cancer patients can wait two months
-just to see a specialist, and waits for problems that are not life-threatening can be half a year. And those who are
-particularly concerned with delays, and can afford it, speed across the border to the United States.
-Chretien is open to charges that he is not the best defender of the health system, since he slashed federal health
-transfers to the provinces by a third in the second half of the 1990s as he sought to balance the federal books.
-"The federal Liberals were the ones who hurt health care more than any other government has done that,"
-Alliance leader Stockwell Day told a news conference in Toronto.
-Health care could help determine whether Chretien can win a third parliamentary majority on election day, Nov.
-27, pushing aside an Alliance surge in the public opinion polls during the first week of the campaign. Health care
-ranks at the top of voters' concerns in most polls.
-Day denies the Alliance would implement a two-tier system, but how far the party would go toward allowing a
-greater role for private health care remained unclear.
-In fact, privatised health care already exists in Canada. One third of health costs - especially drugs, home care
-and physiotherapy - are already paid by patients or by insurance.
-This year, the government of Alberta, where Day was finance minister before moving to the Alliance, enacted
-legislation that will allow the government to pay private clinics to offer services free of charge.
-The Chretien government did not stop Alberta, and Day said on Tuesday he would be open to the Alberta model
-on a national basis if services were provided free, with no jumping to the head of the line.
-It is a big leap from that, where in theory wealth does not buy quicker service, to the British system where it does.
-The Alliance platform does not speak of private care, but Day's campaign co-chairman, Jason Kenney, seemed to
-allow for that possibility, during a recent CBC television programme when he said people should have choices.
-Page 88 of 163 © 2021 Factiva, Inc. All rights reserved.
-"You can have a quality universal public health-care system available to all, everyone, and allow some people
-some choices, like, for instance, every Western European country does," he said. "But that would be up to the
-provinces as long as the federal government would guarantee that not a single person goes without quality care
-because they can afford it."
-Alliance deputy leader Deb Grey, asked on CBC on Wednesday if Kenney made a mistake, said: "No, not at all."
-She pointed out that it was because of the government that 200,000 of Canada's 30 million people were on
-waiting lists.
-However, Kenney's comments drew venom from all four of the other main parties, with most making the
-comparison not with Europe but with the United States.</t>
+    <t>Male Central (out of 5) - Rafael</t>
   </si>
   <si>
     <t>Female Central (out of 5) - Rafael</t>
-  </si>
-  <si>
-    <t>Male Central (out of 5) - Rafael</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -4396,9 +3720,9 @@
   </sheetPr>
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F96" sqref="F96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4442,10 +3766,10 @@
         <v>8</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>210</v>
+        <v>181</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>211</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -7424,439 +6748,169 @@
       </c>
     </row>
     <row r="87" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="4">
-        <v>86</v>
-      </c>
-      <c r="B87" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C87" s="4">
-        <v>2000</v>
-      </c>
-      <c r="D87" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E87" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="F87" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="G87" s="4">
-        <v>1</v>
-      </c>
-      <c r="H87" s="4">
-        <v>5</v>
-      </c>
-      <c r="I87" s="4">
-        <v>4</v>
-      </c>
+      <c r="A87" s="4"/>
+      <c r="B87" s="5"/>
+      <c r="C87" s="4"/>
+      <c r="D87" s="5"/>
+      <c r="E87" s="6"/>
+      <c r="F87" s="7"/>
+      <c r="G87" s="4"/>
+      <c r="H87" s="4"/>
+      <c r="I87" s="4"/>
     </row>
     <row r="88" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="4">
-        <v>87</v>
-      </c>
-      <c r="B88" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C88" s="4">
-        <v>2000</v>
-      </c>
-      <c r="D88" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E88" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="F88" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="G88" s="4">
-        <v>1</v>
-      </c>
-      <c r="H88" s="4">
-        <v>5</v>
-      </c>
-      <c r="I88" s="4">
-        <v>4</v>
-      </c>
+      <c r="A88" s="4"/>
+      <c r="B88" s="5"/>
+      <c r="C88" s="4"/>
+      <c r="D88" s="5"/>
+      <c r="E88" s="6"/>
+      <c r="F88" s="7"/>
+      <c r="G88" s="4"/>
+      <c r="H88" s="4"/>
+      <c r="I88" s="4"/>
     </row>
     <row r="89" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="4">
-        <v>88</v>
-      </c>
-      <c r="B89" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C89" s="4">
-        <v>2000</v>
-      </c>
-      <c r="D89" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E89" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="F89" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="G89" s="4">
-        <v>2</v>
-      </c>
-      <c r="H89" s="4">
-        <v>5</v>
-      </c>
-      <c r="I89" s="4">
-        <v>4</v>
-      </c>
+      <c r="A89" s="4"/>
+      <c r="B89" s="5"/>
+      <c r="C89" s="4"/>
+      <c r="D89" s="5"/>
+      <c r="E89" s="6"/>
+      <c r="F89" s="7"/>
+      <c r="G89" s="4"/>
+      <c r="H89" s="4"/>
+      <c r="I89" s="4"/>
     </row>
     <row r="90" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="4">
-        <v>89</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C90" s="4">
-        <v>2000</v>
-      </c>
-      <c r="D90" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E90" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="F90" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="G90" s="4">
-        <v>1</v>
-      </c>
-      <c r="H90" s="4">
-        <v>5</v>
-      </c>
-      <c r="I90" s="4">
-        <v>4</v>
-      </c>
+      <c r="A90" s="4"/>
+      <c r="B90" s="5"/>
+      <c r="C90" s="4"/>
+      <c r="D90" s="5"/>
+      <c r="E90" s="6"/>
+      <c r="F90" s="7"/>
+      <c r="G90" s="4"/>
+      <c r="H90" s="4"/>
+      <c r="I90" s="4"/>
     </row>
     <row r="91" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="4">
-        <v>90</v>
-      </c>
-      <c r="B91" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C91" s="4">
-        <v>2000</v>
-      </c>
-      <c r="D91" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E91" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="F91" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="G91" s="4">
-        <v>1</v>
-      </c>
-      <c r="H91" s="4">
-        <v>5</v>
-      </c>
-      <c r="I91" s="4">
-        <v>5</v>
-      </c>
+      <c r="A91" s="4"/>
+      <c r="B91" s="5"/>
+      <c r="C91" s="4"/>
+      <c r="D91" s="5"/>
+      <c r="E91" s="6"/>
+      <c r="F91" s="7"/>
+      <c r="G91" s="4"/>
+      <c r="H91" s="4"/>
+      <c r="I91" s="4"/>
     </row>
     <row r="92" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="4">
-        <v>91</v>
-      </c>
-      <c r="B92" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C92" s="4">
-        <v>2000</v>
-      </c>
-      <c r="D92" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E92" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="F92" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="G92" s="4">
-        <v>1</v>
-      </c>
-      <c r="H92" s="4">
-        <v>5</v>
-      </c>
-      <c r="I92" s="4">
-        <v>5</v>
-      </c>
+      <c r="A92" s="4"/>
+      <c r="B92" s="5"/>
+      <c r="C92" s="4"/>
+      <c r="D92" s="5"/>
+      <c r="E92" s="6"/>
+      <c r="F92" s="7"/>
+      <c r="G92" s="4"/>
+      <c r="H92" s="4"/>
+      <c r="I92" s="4"/>
     </row>
     <row r="93" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="4">
-        <v>92</v>
-      </c>
-      <c r="B93" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C93" s="4">
-        <v>2000</v>
-      </c>
-      <c r="D93" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E93" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="F93" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="G93" s="4">
-        <v>1</v>
-      </c>
-      <c r="H93" s="4">
-        <v>5</v>
-      </c>
-      <c r="I93" s="4">
-        <v>4</v>
-      </c>
+      <c r="A93" s="4"/>
+      <c r="B93" s="5"/>
+      <c r="C93" s="4"/>
+      <c r="D93" s="5"/>
+      <c r="E93" s="6"/>
+      <c r="F93" s="7"/>
+      <c r="G93" s="4"/>
+      <c r="H93" s="4"/>
+      <c r="I93" s="4"/>
     </row>
     <row r="94" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="4">
-        <v>93</v>
-      </c>
-      <c r="B94" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C94" s="4">
-        <v>2000</v>
-      </c>
-      <c r="D94" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E94" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="F94" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="G94" s="4">
-        <v>2</v>
-      </c>
-      <c r="H94" s="4">
-        <v>5</v>
-      </c>
-      <c r="I94" s="4">
-        <v>5</v>
-      </c>
+      <c r="A94" s="4"/>
+      <c r="B94" s="5"/>
+      <c r="C94" s="4"/>
+      <c r="D94" s="5"/>
+      <c r="E94" s="6"/>
+      <c r="F94" s="7"/>
+      <c r="G94" s="4"/>
+      <c r="H94" s="4"/>
+      <c r="I94" s="4"/>
     </row>
     <row r="95" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="4">
-        <v>94</v>
-      </c>
-      <c r="B95" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C95" s="4">
-        <v>2000</v>
-      </c>
-      <c r="D95" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E95" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="F95" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="G95" s="4">
-        <v>3</v>
-      </c>
-      <c r="H95" s="4">
-        <v>5</v>
-      </c>
-      <c r="I95" s="4">
-        <v>4</v>
-      </c>
+      <c r="A95" s="4"/>
+      <c r="B95" s="5"/>
+      <c r="C95" s="4"/>
+      <c r="D95" s="5"/>
+      <c r="E95" s="6"/>
+      <c r="F95" s="7"/>
+      <c r="G95" s="4"/>
+      <c r="H95" s="4"/>
+      <c r="I95" s="4"/>
     </row>
     <row r="96" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="4">
-        <v>95</v>
-      </c>
-      <c r="B96" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C96" s="4">
-        <v>2000</v>
-      </c>
-      <c r="D96" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E96" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="F96" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="G96" s="4">
-        <v>1</v>
-      </c>
-      <c r="H96" s="4">
-        <v>4</v>
-      </c>
-      <c r="I96" s="4">
-        <v>5</v>
-      </c>
+      <c r="A96" s="4"/>
+      <c r="B96" s="5"/>
+      <c r="C96" s="4"/>
+      <c r="D96" s="5"/>
+      <c r="E96" s="6"/>
+      <c r="F96" s="7"/>
+      <c r="G96" s="4"/>
+      <c r="H96" s="4"/>
+      <c r="I96" s="4"/>
     </row>
     <row r="97" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="4">
-        <v>96</v>
-      </c>
-      <c r="B97" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C97" s="4">
-        <v>2000</v>
-      </c>
-      <c r="D97" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E97" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="F97" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="G97" s="4">
-        <v>1</v>
-      </c>
-      <c r="H97" s="4">
-        <v>5</v>
-      </c>
-      <c r="I97" s="4">
-        <v>4</v>
-      </c>
+      <c r="A97" s="4"/>
+      <c r="B97" s="5"/>
+      <c r="C97" s="4"/>
+      <c r="D97" s="5"/>
+      <c r="E97" s="7"/>
+      <c r="F97" s="7"/>
+      <c r="G97" s="4"/>
+      <c r="H97" s="4"/>
+      <c r="I97" s="4"/>
     </row>
     <row r="98" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="4">
-        <v>97</v>
-      </c>
-      <c r="B98" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C98" s="4">
-        <v>2000</v>
-      </c>
-      <c r="D98" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E98" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="F98" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="G98" s="4">
-        <v>1</v>
-      </c>
-      <c r="H98" s="4">
-        <v>4</v>
-      </c>
-      <c r="I98" s="4">
-        <v>5</v>
-      </c>
+      <c r="A98" s="4"/>
+      <c r="B98" s="5"/>
+      <c r="C98" s="4"/>
+      <c r="D98" s="5"/>
+      <c r="E98" s="6"/>
+      <c r="F98" s="7"/>
+      <c r="G98" s="4"/>
+      <c r="H98" s="4"/>
+      <c r="I98" s="4"/>
     </row>
     <row r="99" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="4">
-        <v>98</v>
-      </c>
-      <c r="B99" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C99" s="4">
-        <v>2000</v>
-      </c>
-      <c r="D99" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E99" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="F99" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="G99" s="4">
-        <v>1</v>
-      </c>
-      <c r="H99" s="4">
-        <v>5</v>
-      </c>
-      <c r="I99" s="4">
-        <v>3</v>
-      </c>
+      <c r="A99" s="4"/>
+      <c r="B99" s="5"/>
+      <c r="C99" s="4"/>
+      <c r="D99" s="5"/>
+      <c r="E99" s="6"/>
+      <c r="F99" s="7"/>
+      <c r="G99" s="4"/>
+      <c r="H99" s="4"/>
+      <c r="I99" s="4"/>
     </row>
     <row r="100" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="4">
-        <v>99</v>
-      </c>
-      <c r="B100" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C100" s="4">
-        <v>2000</v>
-      </c>
-      <c r="D100" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E100" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="F100" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="G100" s="4">
-        <v>1</v>
-      </c>
-      <c r="H100" s="4">
-        <v>4</v>
-      </c>
-      <c r="I100" s="4">
-        <v>4</v>
-      </c>
+      <c r="A100" s="4"/>
+      <c r="B100" s="5"/>
+      <c r="C100" s="4"/>
+      <c r="D100" s="5"/>
+      <c r="E100" s="6"/>
+      <c r="F100" s="7"/>
+      <c r="G100" s="4"/>
+      <c r="H100" s="4"/>
+      <c r="I100" s="4"/>
     </row>
     <row r="101" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="4">
-        <v>100</v>
-      </c>
-      <c r="B101" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C101" s="4">
-        <v>2000</v>
-      </c>
-      <c r="D101" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E101" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="F101" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="G101" s="4">
-        <v>1</v>
-      </c>
-      <c r="H101" s="4">
-        <v>5</v>
-      </c>
-      <c r="I101" s="4">
-        <v>5</v>
-      </c>
+      <c r="A101" s="4"/>
+      <c r="B101" s="5"/>
+      <c r="C101" s="4"/>
+      <c r="D101" s="5"/>
+      <c r="E101" s="6"/>
+      <c r="F101" s="7"/>
+      <c r="G101" s="4"/>
+      <c r="H101" s="4"/>
+      <c r="I101" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>